<commit_message>
Finished implementing Integration Tests
</commit_message>
<xml_diff>
--- a/Project Testing.xlsx
+++ b/Project Testing.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoinaru/Personal/Arnia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoinaru/Personal/Arnia/UnitTestingPlayground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC69158-E8BF-6944-ACB9-D3D76363FFBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EF0DE-7282-884C-837D-E3216A5FFD26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31760" yWindow="2800" windowWidth="23040" windowHeight="17440" xr2:uid="{2750F1FB-6C4F-6E48-BA68-911D858F5DBE}"/>
+    <workbookView xWindow="30660" yWindow="3700" windowWidth="23040" windowHeight="17440" xr2:uid="{2750F1FB-6C4F-6E48-BA68-911D858F5DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ref" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="ImplemStatus">ref!$A$1:$A$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
   <si>
     <t>Unit</t>
   </si>
@@ -205,6 +209,15 @@
   </si>
   <si>
     <t>Valid userId and token</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>Not Implemented</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -257,7 +270,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -567,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F5366A-9A2A-8F49-AAAE-922E4504FF81}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D19"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,17 +623,21 @@
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -602,8 +650,11 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -616,24 +667,33 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -643,24 +703,33 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -670,40 +739,55 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -716,16 +800,22 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>28</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -735,32 +825,44 @@
       <c r="D16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -773,8 +875,11 @@
       <c r="D20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -787,32 +892,44 @@
       <c r="D21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>43</v>
       </c>
       <c r="D23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>46</v>
       </c>
@@ -822,24 +939,33 @@
       <c r="D25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>49</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>51</v>
       </c>
@@ -849,32 +975,44 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>41</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>43</v>
       </c>
       <c r="D30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>53</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>55</v>
       </c>
@@ -884,29 +1022,41 @@
       <c r="D32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>43</v>
       </c>
       <c r="D34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>53</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -914,6 +1064,44 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:D19"/>
   </mergeCells>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Implemented">
+      <formula>NOT(ISERROR(SEARCH("Implemented",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Not Implemented">
+      <formula>NOT(ISERROR(SEARCH("Not Implemented",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E35" xr:uid="{6AA73A4C-DA2A-AD44-908D-0E6D2BA01327}">
+      <formula1>ImplemStatus</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A06B44E-AB5F-3E4C-B9EA-1607E02B7BED}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>